<commit_message>
Made multi-matrix hardware fixed software support
</commit_message>
<xml_diff>
--- a/Fonts/FontHelper.xlsx
+++ b/Fonts/FontHelper.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="182">
   <si>
     <t>A</t>
   </si>
@@ -565,6 +565,12 @@
   </si>
   <si>
     <t>Font 1</t>
+  </si>
+  <si>
+    <t>{0,4,4,4,4,4,4,28}</t>
+  </si>
+  <si>
+    <t>{0,0,8,0,8,8,10,4}</t>
   </si>
 </sst>
 </file>
@@ -904,7 +910,7 @@
   <dimension ref="C2:AD37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <f>C4+2*D4+4*E4+8*F4+G4*16+H4*32+I4*64+J4*128</f>
+        <f t="shared" ref="L4:L11" si="0">C4+2*D4+4*E4+8*F4+G4*16+H4*32+I4*64+J4*128</f>
         <v>0</v>
       </c>
       <c r="N4" s="1" t="str">
@@ -955,31 +961,31 @@
         <v/>
       </c>
       <c r="O4" s="1" t="str">
-        <f t="shared" ref="O4:U11" si="0">IF(D4=1,8,"")</f>
+        <f t="shared" ref="O4:U11" si="1">IF(D4=1,8,"")</f>
         <v/>
       </c>
       <c r="P4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V4" s="2"/>
@@ -1010,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1028,39 +1034,39 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f>C5+2*D5+4*E5+8*F5+G5*16+H5*32+I5*64+J5*128</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="N5" s="1" t="str">
-        <f t="shared" ref="N5:N11" si="1">IF(C5=1,8,"")</f>
+        <f t="shared" ref="N5:N11" si="2">IF(C5=1,8,"")</f>
         <v/>
       </c>
       <c r="O5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P5" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
       <c r="Q5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V5" s="2"/>
@@ -1088,14 +1094,14 @@
         <v>0</v>
       </c>
       <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
@@ -1109,39 +1115,39 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <f>C6+2*D6+4*E6+8*F6+G6*16+H6*32+I6*64+J6*128</f>
-        <v>6</v>
-      </c>
-      <c r="N6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O6" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="P6" s="1">
-        <f t="shared" si="0"/>
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="Q6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="R6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V6" s="2"/>
@@ -1172,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1190,39 +1196,39 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <f>C7+2*D7+4*E7+8*F7+G7*16+H7*32+I7*64+J7*128</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="N7" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="O7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P7" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
       <c r="Q7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V7" s="2"/>
@@ -1253,11 +1259,11 @@
         <v>0</v>
       </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
         <v>0</v>
       </c>
@@ -1271,39 +1277,39 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <f>C8+2*D8+4*E8+8*F8+G8*16+H8*32+I8*64+J8*128</f>
-        <v>4</v>
-      </c>
-      <c r="N8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P8" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="Q8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="R8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V8" s="2"/>
@@ -1334,11 +1340,11 @@
         <v>0</v>
       </c>
       <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9">
         <v>0</v>
       </c>
@@ -1352,39 +1358,39 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <f>C9+2*D9+4*E9+8*F9+G9*16+H9*32+I9*64+J9*128</f>
-        <v>4</v>
-      </c>
-      <c r="N9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="Q9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="R9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V9" s="2"/>
@@ -1412,14 +1418,14 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
       <c r="G10">
         <v>0</v>
       </c>
@@ -1433,39 +1439,39 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <f>C10+2*D10+4*E10+8*F10+G10*16+H10*32+I10*64+J10*128</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="Q10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="P10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="R10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V10" s="2"/>
@@ -1493,13 +1499,13 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1514,39 +1520,39 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <f>C11+2*D11+4*E11+8*F11+G11*16+H11*32+I11*64+J11*128</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="N11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="P11" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Q11" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
+      <c r="Q11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
       <c r="R11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V11" s="2"/>
@@ -1616,7 +1622,7 @@
       </c>
       <c r="L13" t="str">
         <f>CONCATENATE("{",L4,",",L5,",",L6,",",L7,",",L8,",",L9,",",L10,",",L11,"}")</f>
-        <v>{0,4,6,4,4,4,4,14}</v>
+        <v>{0,0,8,0,8,8,10,4}</v>
       </c>
       <c r="W13" s="3" t="s">
         <v>61</v>
@@ -1678,7 +1684,7 @@
         <v>89</v>
       </c>
       <c r="AD14" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="3:30" x14ac:dyDescent="0.25">
@@ -1760,7 +1766,7 @@
         <v>11</v>
       </c>
       <c r="AA16" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="AC16" t="s">
         <v>91</v>
@@ -2242,7 +2248,7 @@
     <row r="37" spans="23:30" x14ac:dyDescent="0.25">
       <c r="W37" t="str">
         <f>CONCATENATE("{",X4,",",X5,",",X6,",",X7,",",X8,",",X9,",",X10,",",X11,",",X12,",",X13,",",X14,",",X15,",",X16,",",X17,",",X18,",",X19,",",X20,",",X21,",",X22,",",X23,",",X24,",",X25,",",X26,",",X27,",",X28,",",X29,",",X30,",",X31,",",X32,",",X33,",",X34,",",X35,",",AA4,",",AA5,",",AA6,",",AA7,",",AA8,",",AA9,",",AA10,",",AA11,",",AA12,",",AA13,",",AA14,",",AA15,",",AA16,",",AA17,",",AA18,",",AA19,",",AA20,",",AA21,",",AA22,",",AA23,",",AA24,",",AA25,",",AA26,",",AA27,",",AA28,",",AA29,",",AA30,",",AA31,",",AA32,",",AA33,",",AA34,",",AA35,",",AD4,",",AD5,",",AD6,",",AD7,",",AD8,",",AD9,",",AD10,",",AD11,",",AD12,",",AD13,",",AD14,",",AD15,",",AD16,",",AD17,",",AD18,",",AD19,",",AD20,",",AD21,",",AD22,",",AD23,",",AD24,",",AD25,",",AD26,",",AD27,",",AD28,",",AD29,",",AD30,",",AD31,",",AD32,",",AD33,",",AD34,"}",";")</f>
-        <v>{{0,0,0,0,0,0,0,0},{0,4,4,4,4,4,0,4},{0,10,10,10,0,0,0,0},{0,0,10,31,10,31,10,0},{0,4,30,1,14,16,15,4},{0,2,21,10,4,10,21,8},{0,6,9,9,6,21,9,22},{0,4,4,4,0,0,0,0},{0,16,8,8,8,8,8,16},{0,4,8,8,8,8,8,4},{0,0,8,28,8,28,8,0},{0,0,8,8,62,8,8,0},{0,0,0,0,0,8,8,4},{0,0,0,0,62,0,0,0},{0,0,0,0,0,0,12,12},{0,16,8,12,4,6,2,1},{0,14,25,29,21,23,19,14},{0,4,6,4,4,4,4,14},{0,14,17,16,8,4,2,31},{0,14,17,16,14,16,17,14},{0,8,12,10,31,8,8,8},{0,31,1,1,15,16,17,14},{0,14,17,1,15,17,17,14},{0,31,16,8,4,4,2,2},{0,14,17,17,14,17,17,14},{0,14,17,17,30,16,17,14},{0,0,6,6,0,6,6,0},{0,0,6,6,0,4,6,2},{0,8,4,2,1,2,4,8},{0,0,0,31,0,31,0,0},{0,4,8,16,32,16,8,4},{0,14,17,16,12,4,0,4},{0,14,17,21,21,29,1,30},{0,14,17,17,31,17,17,17},{0,15,17,17,15,17,17,15},{0,14,17,1,1,1,17,14},{0,15,17,17,17,17,17,15},{0,31,1,1,15,1,1,31},{0,31,1,1,15,1,1,1},{0,14,17,1,25,17,17,14},{0,17,17,17,31,17,17,17},{0,31,4,4,4,4,4,31},{0,31,4,4,4,4,5,2},{0,17,9,5,3,5,9,17},{0,4,4,4,4,4,4,8},{0,17,27,21,17,17,17,17},{0,17,19,19,21,25,25,17},{0,14,17,17,17,17,17,14},{0,15,17,17,15,1,1,1},{0,14,17,17,17,21,25,30},{0,15,17,17,15,5,9,17},{0,14,17,1,14,16,17,14},{0,31,4,4,4,4,4,4},{0,17,17,17,17,17,17,14},{0,17,17,17,17,10,10,4},{0,17,17,17,17,21,27,17},{0,17,17,10,4,10,17,17},{0,17,17,10,4,4,4,4},{0,31,16,8,4,2,1,31},{0,14,2,2,2,2,2,14},{0,1,2,6,4,12,8,16},{0,14,8,8,8,8,8,12},{0,4,10,17,0,0,0,0},{0,0,0,0,0,0,0,31},{0,1,2,4,0,0,0,0},{0,0,0,14,16,30,17,30},{0,1,1,1,15,17,17,15},{0,0,0,14,17,1,17,14},{0,16,16,16,30,17,17,30},{0,0,0,14,17,31,1,14},{0,8,20,4,14,4,4,4},{0,0,0,30,17,30,16,14},{0,1,1,1,15,17,17,17},{0,0,0,4,0,4,4,4},{0,0,0,4,0,4,4,2},{0,1,1,9,5,3,5,9},{0,4,4,4,4,4,4,8},{0,0,0,11,21,21,21,21},{0,0,0,14,18,18,18,18},{0,0,0,14,17,17,17,14},{0,0,0,15,17,15,1,1},{0,0,0,30,17,30,16,16},{0,0,0,15,17,1,1,1},{0,0,0,30,1,14,16,15},{0,4,4,14,4,4,4,8},{0,0,0,17,17,17,17,30},{0,0,0,17,17,17,10,4},{0,0,0,17,21,21,21,10},{0,0,0,17,10,4,10,17},{0,0,0,17,17,30,16,14},{0,0,0,31,8,4,2,31},{0,24,4,4,2,4,4,24},{0,4,4,4,4,4,4,4},{0,6,8,8,16,8,8,6},{0,0,0,9,21,18,0,0}};</v>
+        <v>{{0,0,0,0,0,0,0,0},{0,4,4,4,4,4,0,4},{0,10,10,10,0,0,0,0},{0,0,10,31,10,31,10,0},{0,4,30,1,14,16,15,4},{0,2,21,10,4,10,21,8},{0,6,9,9,6,21,9,22},{0,4,4,4,0,0,0,0},{0,16,8,8,8,8,8,16},{0,4,8,8,8,8,8,4},{0,0,8,28,8,28,8,0},{0,0,8,8,62,8,8,0},{0,0,0,0,0,8,8,4},{0,0,0,0,62,0,0,0},{0,0,0,0,0,0,12,12},{0,16,8,12,4,6,2,1},{0,14,25,29,21,23,19,14},{0,4,6,4,4,4,4,14},{0,14,17,16,8,4,2,31},{0,14,17,16,14,16,17,14},{0,8,12,10,31,8,8,8},{0,31,1,1,15,16,17,14},{0,14,17,1,15,17,17,14},{0,31,16,8,4,4,2,2},{0,14,17,17,14,17,17,14},{0,14,17,17,30,16,17,14},{0,0,6,6,0,6,6,0},{0,0,6,6,0,4,6,2},{0,8,4,2,1,2,4,8},{0,0,0,31,0,31,0,0},{0,4,8,16,32,16,8,4},{0,14,17,16,12,4,0,4},{0,14,17,21,21,29,1,30},{0,14,17,17,31,17,17,17},{0,15,17,17,15,17,17,15},{0,14,17,1,1,1,17,14},{0,15,17,17,17,17,17,15},{0,31,1,1,15,1,1,31},{0,31,1,1,15,1,1,1},{0,14,17,1,25,17,17,14},{0,17,17,17,31,17,17,17},{0,31,4,4,4,4,4,31},{0,31,4,4,4,4,5,2},{0,17,9,5,3,5,9,17},{0,4,4,4,4,4,4,28},{0,17,27,21,17,17,17,17},{0,17,19,19,21,25,25,17},{0,14,17,17,17,17,17,14},{0,15,17,17,15,1,1,1},{0,14,17,17,17,21,25,30},{0,15,17,17,15,5,9,17},{0,14,17,1,14,16,17,14},{0,31,4,4,4,4,4,4},{0,17,17,17,17,17,17,14},{0,17,17,17,17,10,10,4},{0,17,17,17,17,21,27,17},{0,17,17,10,4,10,17,17},{0,17,17,10,4,4,4,4},{0,31,16,8,4,2,1,31},{0,14,2,2,2,2,2,14},{0,1,2,6,4,12,8,16},{0,14,8,8,8,8,8,12},{0,4,10,17,0,0,0,0},{0,0,0,0,0,0,0,31},{0,1,2,4,0,0,0,0},{0,0,0,14,16,30,17,30},{0,1,1,1,15,17,17,15},{0,0,0,14,17,1,17,14},{0,16,16,16,30,17,17,30},{0,0,0,14,17,31,1,14},{0,8,20,4,14,4,4,4},{0,0,0,30,17,30,16,14},{0,1,1,1,15,17,17,17},{0,0,0,4,0,4,4,4},{0,0,8,0,8,8,10,4},{0,1,1,9,5,3,5,9},{0,4,4,4,4,4,4,8},{0,0,0,11,21,21,21,21},{0,0,0,14,18,18,18,18},{0,0,0,14,17,17,17,14},{0,0,0,15,17,15,1,1},{0,0,0,30,17,30,16,16},{0,0,0,15,17,1,1,1},{0,0,0,30,1,14,16,15},{0,4,4,14,4,4,4,8},{0,0,0,17,17,17,17,30},{0,0,0,17,17,17,10,4},{0,0,0,17,21,21,21,10},{0,0,0,17,10,4,10,17},{0,0,0,17,17,30,16,14},{0,0,0,31,8,4,2,31},{0,24,4,4,2,4,4,24},{0,4,4,4,4,4,4,4},{0,6,8,8,16,8,8,6},{0,0,0,9,21,18,0,0}};</v>
       </c>
     </row>
   </sheetData>

</xml_diff>